<commit_message>
Update local from hosting
</commit_message>
<xml_diff>
--- a/assets/uploads/template_mahasiswa_new.xlsx
+++ b/assets/uploads/template_mahasiswa_new.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_325A5BD4B3C779BFC68E482BCA9B997501EE8BA9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E68ADF1B-28E4-4FC1-A1EE-C2009392D754}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -19,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Nama Lengkap</t>
   </si>
@@ -27,90 +37,37 @@
     <t>NPM</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
     <t>PRODI ID</t>
   </si>
   <si>
-    <t>Alamat</t>
-  </si>
-  <si>
-    <t>Tanggal Lahir</t>
-  </si>
-  <si>
-    <t>No Hp</t>
-  </si>
-  <si>
-    <t>9a94e137-bab8-11eb-a91e-0cc47abcfaa6</t>
-  </si>
-  <si>
-    <t>Natar</t>
-  </si>
-  <si>
-    <t>1995-08-18</t>
-  </si>
-  <si>
-    <t>1996-08-18</t>
-  </si>
-  <si>
     <t>Agung Hardiyanto</t>
   </si>
   <si>
-    <t>agunghardiyanto12@gmail.com</t>
-  </si>
-  <si>
-    <t>Pesawaran</t>
-  </si>
-  <si>
-    <t>08123456789</t>
+    <t>800d3121-f2f9-11eb-8c3d-0cc47abcfaa6</t>
   </si>
   <si>
     <t>Jution Candra Kirana</t>
   </si>
   <si>
-    <t>jutionck@gmail.com</t>
-  </si>
-  <si>
-    <t>081398376227</t>
-  </si>
-  <si>
     <t>Adriyan Lumban Tobing</t>
   </si>
   <si>
-    <t>adrian@gmail.com</t>
-  </si>
-  <si>
-    <t>Natar Lampung</t>
-  </si>
-  <si>
-    <t>081398376226</t>
-  </si>
-  <si>
-    <t>Jenis Kelamin</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>P</t>
+    <t>Ria Setya Handayani</t>
+  </si>
+  <si>
+    <t>8f5585b1-f2f9-11eb-8c3d-0cc47abcfaa6</t>
+  </si>
+  <si>
+    <t>Ayu Futri Batara</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -133,18 +90,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -203,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -255,7 +207,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -449,32 +401,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,106 +432,63 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2">
         <v>13753001</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>13753030</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>13753004</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
+      <c r="B5">
+        <v>13755001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>13755002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>